<commit_message>
repo should be working now
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\StudioProjects\odkVaccine\app\config\assets\framework\forms\framework\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="4020" yWindow="0" windowWidth="24300" windowHeight="17100" firstSheet="1" activeTab="3"/>
   </bookViews>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="93">
   <si>
     <t>comments</t>
   </si>
@@ -295,6 +300,12 @@
   </si>
   <si>
     <t>'?' + opendatakit.getHashString('../config/tables/household/forms/household/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../config/tables/VaccineManager/forms/VaccineManager/',null)</t>
+  </si>
+  <si>
+    <t>VaccineManager</t>
   </si>
 </sst>
 </file>
@@ -524,6 +535,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -822,13 +836,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -836,7 +850,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -853,24 +867,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="101.1640625" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
-    <col min="4" max="4" width="46.1640625" customWidth="1"/>
+    <col min="2" max="2" width="101.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="46.140625" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" customWidth="1"/>
-    <col min="8" max="8" width="31.5" customWidth="1"/>
-    <col min="9" max="9" width="22.1640625" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1">
+    <row r="1" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -897,7 +911,7 @@
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>20</v>
       </c>
@@ -906,7 +920,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="17.5" customHeight="1">
+    <row r="3" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>24</v>
       </c>
@@ -917,13 +931,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>2</v>
       </c>
@@ -934,23 +948,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>67</v>
@@ -962,20 +976,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
         <v>68</v>
@@ -987,20 +1001,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17.25" customHeight="1">
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="59.25" customHeight="1">
+    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
         <v>69</v>
@@ -1012,20 +1026,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17.25" customHeight="1">
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.5" customHeight="1">
+    <row r="17" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="59.25" customHeight="1">
+    <row r="18" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
         <v>70</v>
@@ -1037,20 +1051,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.25" customHeight="1">
+    <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.5" customHeight="1">
+    <row r="20" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="66" customHeight="1">
+    <row r="21" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
         <v>71</v>
@@ -1062,19 +1076,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17.25" customHeight="1">
+    <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.5" customHeight="1">
+    <row r="23" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="66" customHeight="1">
+    <row r="24" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
         <v>72</v>
@@ -1086,19 +1100,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17.25" customHeight="1">
+    <row r="25" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.5" customHeight="1">
+    <row r="26" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="66" customHeight="1">
+    <row r="27" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
         <v>90</v>
@@ -1110,19 +1124,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17.25" customHeight="1">
+    <row r="28" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17.5" customHeight="1">
+    <row r="29" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="66" customHeight="1">
+    <row r="30" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
         <v>73</v>
@@ -1134,19 +1148,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17.25" customHeight="1">
+    <row r="31" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17.5" customHeight="1">
+    <row r="32" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="66" customHeight="1">
+    <row r="33" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
         <v>74</v>
@@ -1158,19 +1172,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17.25" customHeight="1">
+    <row r="34" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17.5" customHeight="1">
+    <row r="35" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="66" customHeight="1">
+    <row r="36" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
         <v>75</v>
@@ -1182,19 +1196,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17.25" customHeight="1">
+    <row r="37" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17.5" customHeight="1">
+    <row r="38" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="66" customHeight="1">
+    <row r="39" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
         <v>76</v>
@@ -1206,19 +1220,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17.25" customHeight="1">
+    <row r="40" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17.5" customHeight="1">
+    <row r="41" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="66" customHeight="1">
+    <row r="42" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
         <v>77</v>
@@ -1230,19 +1244,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17.25" customHeight="1">
+    <row r="43" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17.5" customHeight="1">
+    <row r="44" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="66" customHeight="1">
+    <row r="45" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
         <v>78</v>
@@ -1254,19 +1268,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="17.25" customHeight="1">
+    <row r="46" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="17.5" customHeight="1">
+    <row r="47" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="66" customHeight="1">
+    <row r="48" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
         <v>79</v>
@@ -1278,19 +1292,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="17.25" customHeight="1">
+    <row r="49" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="17.5" customHeight="1">
+    <row r="50" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="66" customHeight="1">
+    <row r="51" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
         <v>80</v>
@@ -1302,19 +1316,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="17.25" customHeight="1">
+    <row r="52" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="17.5" customHeight="1">
+    <row r="53" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="66" customHeight="1">
+    <row r="54" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
         <v>81</v>
@@ -1326,19 +1340,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="17.25" customHeight="1">
+    <row r="55" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="17.5" customHeight="1">
+    <row r="56" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="66" customHeight="1">
+    <row r="57" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
         <v>82</v>
@@ -1350,19 +1364,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="17.25" customHeight="1">
+    <row r="58" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="17.5" customHeight="1">
+    <row r="59" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="66" customHeight="1">
+    <row r="60" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="4" t="s">
         <v>83</v>
@@ -1374,19 +1388,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="17.25" customHeight="1">
+    <row r="61" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="17.5" customHeight="1">
+    <row r="62" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="66" customHeight="1">
+    <row r="63" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="B63" s="4" t="s">
         <v>84</v>
@@ -1398,19 +1412,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="17.25" customHeight="1">
+    <row r="64" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="17.5" customHeight="1">
+    <row r="65" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="66" customHeight="1">
+    <row r="66" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
       <c r="B66" s="4" t="s">
         <v>85</v>
@@ -1422,19 +1436,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="17.25" customHeight="1">
+    <row r="67" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="17.5" customHeight="1">
+    <row r="68" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="66" customHeight="1">
+    <row r="69" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="4" t="s">
         <v>86</v>
@@ -1446,19 +1460,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="17.25" customHeight="1">
+    <row r="70" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="17.5" customHeight="1">
+    <row r="71" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="66" customHeight="1">
+    <row r="72" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
       <c r="B72" s="4" t="s">
         <v>87</v>
@@ -1470,10 +1484,27 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" t="s">
+    <row r="73" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="3"/>
+      <c r="B74" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E74" t="s">
+        <v>39</v>
+      </c>
+      <c r="G74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1496,13 +1527,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="41.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1519,7 +1550,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>88</v>
       </c>
@@ -1528,7 +1559,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1540,7 +1571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1551,7 +1582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28" customHeight="1">
+    <row r="5" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1565,60 +1596,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1"/>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1"/>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1">
+    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1">
+    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="12.75" customHeight="1">
+    <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1">
+    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1">
+    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1">
+    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:3" ht="12.75" customHeight="1">
+    <row r="25" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
     </row>
   </sheetData>
@@ -1633,20 +1664,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1657,7 +1688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1668,7 +1699,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1679,7 +1710,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1690,7 +1721,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1701,7 +1732,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -1712,7 +1743,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -1723,7 +1754,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1734,7 +1765,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -1745,7 +1776,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1756,7 +1787,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -1767,7 +1798,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -1778,7 +1809,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -1789,7 +1820,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1800,7 +1831,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1811,7 +1842,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -1822,7 +1853,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
@@ -1833,7 +1864,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
@@ -1844,7 +1875,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
@@ -1855,7 +1886,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -1866,7 +1897,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -1877,7 +1908,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1888,7 +1919,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1897,6 +1928,17 @@
       </c>
       <c r="C23" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>